<commit_message>
All test cases are running fine
</commit_message>
<xml_diff>
--- a/TestData/HomeLyfDataSheet.xlsx
+++ b/TestData/HomeLyfDataSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL-PC\Documents\Udemy java class\HomeLyf_API\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72991317-FC8B-4C56-A62B-C561E5BFB7CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D75E007-B5FA-4E2D-BCBB-23F151E4F0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>sxwsfy0ecd@zlorkun.com</t>
   </si>
   <si>
-    <t>rowivar934@fashlend.com</t>
-  </si>
-  <si>
     <t>shiv</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
   </si>
   <si>
     <t>pra@789</t>
+  </si>
+  <si>
+    <t>dorad67121@fryshare.com</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,15 +442,15 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>4446556</v>
@@ -476,7 +476,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -493,7 +493,7 @@
         <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -510,7 +510,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
User end to end done
</commit_message>
<xml_diff>
--- a/TestData/HomeLyfDataSheet.xlsx
+++ b/TestData/HomeLyfDataSheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL-PC\Documents\Udemy java class\HomeLyf_API\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D75E007-B5FA-4E2D-BCBB-23F151E4F0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BECF38-AD74-4658-B4E6-977D9558B647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="QDTAS1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>email</t>
   </si>
@@ -88,12 +89,99 @@
   </si>
   <si>
     <t>dorad67121@fryshare.com</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>depId</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>phoneNubmer</t>
+  </si>
+  <si>
+    <t>designation</t>
+  </si>
+  <si>
+    <t>birthDate</t>
+  </si>
+  <si>
+    <t>Onkar</t>
+  </si>
+  <si>
+    <t>om</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>singal</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>ManualTester</t>
+  </si>
+  <si>
+    <t>joinDate</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Pune</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>kure.onkar41@gmail.com</t>
+  </si>
+  <si>
+    <t>Onkar@41</t>
+  </si>
+  <si>
+    <t>onkark</t>
+  </si>
+  <si>
+    <t>omkar</t>
+  </si>
+  <si>
+    <t>kure</t>
+  </si>
+  <si>
+    <t>Automation.Engineer</t>
+  </si>
+  <si>
+    <t>mayivec121@irnini.com</t>
+  </si>
+  <si>
+    <t>Bebo@123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -132,9 +220,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -418,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,4 +612,164 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E5CA742-98AB-4961-969B-2FA3A42D36F0}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2">
+        <v>1234567890</v>
+      </c>
+      <c r="K2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="2">
+        <v>45334</v>
+      </c>
+      <c r="M2" s="2">
+        <v>45334</v>
+      </c>
+      <c r="N2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3">
+        <v>1234567892</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="2">
+        <v>35994</v>
+      </c>
+      <c r="M3" s="2">
+        <v>43330</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{5E96AF63-817E-4D4A-AC03-4DAA0C8B5496}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{310A2101-DAAD-4792-A19A-149115994858}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{5BD96FA0-B628-455E-9A45-D6A250A221D0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
End to End QDTAS User api Done
</commit_message>
<xml_diff>
--- a/TestData/HomeLyfDataSheet.xlsx
+++ b/TestData/HomeLyfDataSheet.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL-PC\Documents\Udemy java class\HomeLyf_API\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C940CC8-383E-4407-9D8D-9ACD0DD0CE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4654A7-9CE7-4E91-9C6D-7CB1726FAF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="QDTAS1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
   <si>
     <t>email</t>
   </si>
@@ -151,12 +152,6 @@
     <t>male</t>
   </si>
   <si>
-    <t>kure.onkar41@gmail.com</t>
-  </si>
-  <si>
-    <t>Onkar@41</t>
-  </si>
-  <si>
     <t>onkark</t>
   </si>
   <si>
@@ -172,7 +167,25 @@
     <t>Bebo@123</t>
   </si>
   <si>
+    <t>admin@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin@123</t>
+  </si>
+  <si>
     <t>misaxay339@fryshare.com</t>
+  </si>
+  <si>
+    <t>Shiv</t>
+  </si>
+  <si>
+    <t>Shiv@12345</t>
+  </si>
+  <si>
+    <t>shivay@123</t>
+  </si>
+  <si>
+    <t>tiselap800@irnini.com</t>
   </si>
 </sst>
 </file>
@@ -505,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -602,15 +615,34 @@
         <v>19</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>8745235686</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{B56FEB8B-DA39-4E9C-B2DA-B388A7DCF8DB}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{0F89D6F2-51E3-43F9-BBC7-5A465FEB229D}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{F7B0621D-82D0-46F3-8586-5752AE52DF98}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{A7C70BDA-CC56-449F-B6ED-A184B975E275}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{900FE29C-27C8-4259-BD52-E59D6727A128}"/>
+    <hyperlink ref="E6" r:id="rId6" xr:uid="{77DA7855-37B7-433A-A663-38659B0DB43C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -619,7 +651,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,22 +710,22 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
         <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
         <v>40</v>
@@ -708,7 +740,7 @@
         <v>1234567890</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L2" s="2">
         <v>45334</v>
@@ -725,10 +757,10 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
@@ -772,4 +804,16 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0567B51A-D9A7-4356-85AC-A49E8578015A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update data in excel
</commit_message>
<xml_diff>
--- a/TestData/HomeLyfDataSheet.xlsx
+++ b/TestData/HomeLyfDataSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL-PC\Documents\Udemy java class\HomeLyf_API\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE9C35B-AEE6-4F29-80A8-CF4E42E82B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015BBCE2-FF8B-409A-8DDB-BD2CC370C047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -185,7 +185,7 @@
     <t>shivay@123</t>
   </si>
   <si>
-    <t>papoget159@fryshare.com</t>
+    <t>befov86073@hisotyr.com</t>
   </si>
 </sst>
 </file>

</xml_diff>